<commit_message>
Descriptions of A.N. Python procedures.
</commit_message>
<xml_diff>
--- a/an_code_inventory.xlsx
+++ b/an_code_inventory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6920" yWindow="640" windowWidth="30900" windowHeight="17180" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="6920" yWindow="640" windowWidth="30900" windowHeight="17180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="code descriptions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="131">
   <si>
     <t>nir_opt_comp</t>
   </si>
@@ -407,6 +407,12 @@
   </si>
   <si>
     <t>plot_spread.py</t>
+  </si>
+  <si>
+    <t>Same as nir_opt_comp with one exception below:</t>
+  </si>
+  <si>
+    <t>4) Tab-delimited txt file "Exclude_Objs_special.txt" which has list of excluded objects; this is slightly different from "Exclude_Objs_special.txt"</t>
   </si>
 </sst>
 </file>
@@ -503,8 +509,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="141">
+  <cellStyleXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -674,7 +682,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="141">
+  <cellStyles count="143">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -745,6 +753,7 @@
     <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -815,6 +824,7 @@
     <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1146,9 +1156,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1323,7 +1333,7 @@
         <v>32</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>22</v>
+        <v>129</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>22</v>
@@ -1342,11 +1352,13 @@
       </c>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="2:11" ht="45">
+    <row r="9" spans="2:11" ht="75">
       <c r="B9" s="7"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4" t="s">
         <v>55</v>
@@ -1866,7 +1878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>

</xml_diff>